<commit_message>
Add command for check #9.
</commit_message>
<xml_diff>
--- a/hfc_outputs.xlsx
+++ b/hfc_outputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="4650" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="1. incomplete" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="99">
   <si>
     <t>id</t>
   </si>
@@ -147,6 +147,186 @@
   </si>
   <si>
     <t>Michael</t>
+  </si>
+  <si>
+    <t>occupation_other</t>
+  </si>
+  <si>
+    <t>Hair dresser</t>
+  </si>
+  <si>
+    <t>Soccer player</t>
+  </si>
+  <si>
+    <t>Chef at a school</t>
+  </si>
+  <si>
+    <t>Maid</t>
+  </si>
+  <si>
+    <t>Youth Activist</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Research Supervisor</t>
+  </si>
+  <si>
+    <t>Singing</t>
+  </si>
+  <si>
+    <t>Tutoring</t>
+  </si>
+  <si>
+    <t>I create ideas for all company types</t>
+  </si>
+  <si>
+    <t>Studio Producer</t>
+  </si>
+  <si>
+    <t>Worked in a saloon</t>
+  </si>
+  <si>
+    <t>Footballer</t>
+  </si>
+  <si>
+    <t>Waiter</t>
+  </si>
+  <si>
+    <t>Ukutapisha  Amenshi   Pa   Pompi  ya   ba  Care.</t>
+  </si>
+  <si>
+    <t>Entrepreneur</t>
+  </si>
+  <si>
+    <t>Piece work</t>
+  </si>
+  <si>
+    <t>It was voluntary work no pay at all</t>
+  </si>
+  <si>
+    <t>Community work</t>
+  </si>
+  <si>
+    <t>Pre school teacher</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Dramatist</t>
+  </si>
+  <si>
+    <t>Radio personality</t>
+  </si>
+  <si>
+    <t>Hair stylist</t>
+  </si>
+  <si>
+    <t>Hair Stylist</t>
+  </si>
+  <si>
+    <t>I used to work as a laboratory clerk</t>
+  </si>
+  <si>
+    <t>Librarian</t>
+  </si>
+  <si>
+    <t>Co driver</t>
+  </si>
+  <si>
+    <t>Manicure and pedicure</t>
+  </si>
+  <si>
+    <t>Chef</t>
+  </si>
+  <si>
+    <t>Cashier</t>
+  </si>
+  <si>
+    <t>Barman</t>
+  </si>
+  <si>
+    <t>Hairdresser</t>
+  </si>
+  <si>
+    <t>Nothing</t>
+  </si>
+  <si>
+    <t>Secretary</t>
+  </si>
+  <si>
+    <t>Barker</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Depot Clerk</t>
+  </si>
+  <si>
+    <t>Fuel Attendant</t>
+  </si>
+  <si>
+    <t>Taxi driver</t>
+  </si>
+  <si>
+    <t>Supervisor</t>
+  </si>
+  <si>
+    <t>Managing the lodge</t>
+  </si>
+  <si>
+    <t>Radio DJ</t>
+  </si>
+  <si>
+    <t>Teaching grade nine</t>
+  </si>
+  <si>
+    <t>Beer brewing</t>
+  </si>
+  <si>
+    <t>Catering</t>
+  </si>
+  <si>
+    <t>General worker</t>
+  </si>
+  <si>
+    <t>Business lady</t>
+  </si>
+  <si>
+    <t>Grocery shop</t>
+  </si>
+  <si>
+    <t>Sale different things</t>
+  </si>
+  <si>
+    <t>Maid jobs</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Nothing, just house work.</t>
+  </si>
+  <si>
+    <t>Get it from my parents</t>
+  </si>
+  <si>
+    <t>I am a footballer</t>
+  </si>
+  <si>
+    <t>At the moment am just sitted at home</t>
+  </si>
+  <si>
+    <t>Please specify your occupation.</t>
+  </si>
+  <si>
+    <t>Nonmissing specify other value encountered</t>
   </si>
 </sst>
 </file>
@@ -464,7 +644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -1028,7 +1208,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1132,12 +1312,1609 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" t="s">
+        <v>97</v>
+      </c>
+      <c r="E33" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" t="s">
+        <v>97</v>
+      </c>
+      <c r="E36" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" t="s">
+        <v>97</v>
+      </c>
+      <c r="E37" t="s">
+        <v>66</v>
+      </c>
+      <c r="F37" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" t="s">
+        <v>97</v>
+      </c>
+      <c r="E38" t="s">
+        <v>67</v>
+      </c>
+      <c r="F38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" t="s">
+        <v>97</v>
+      </c>
+      <c r="E39" t="s">
+        <v>68</v>
+      </c>
+      <c r="F39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" t="s">
+        <v>97</v>
+      </c>
+      <c r="E41" t="s">
+        <v>70</v>
+      </c>
+      <c r="F41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" t="s">
+        <v>97</v>
+      </c>
+      <c r="E42" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" t="s">
+        <v>97</v>
+      </c>
+      <c r="E44" t="s">
+        <v>61</v>
+      </c>
+      <c r="F44" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" t="s">
+        <v>97</v>
+      </c>
+      <c r="E45" t="s">
+        <v>72</v>
+      </c>
+      <c r="F45" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" t="s">
+        <v>97</v>
+      </c>
+      <c r="E46" t="s">
+        <v>73</v>
+      </c>
+      <c r="F46" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" t="s">
+        <v>97</v>
+      </c>
+      <c r="E47" t="s">
+        <v>74</v>
+      </c>
+      <c r="F47" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" t="s">
+        <v>97</v>
+      </c>
+      <c r="E48" t="s">
+        <v>75</v>
+      </c>
+      <c r="F48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" t="s">
+        <v>97</v>
+      </c>
+      <c r="E49" t="s">
+        <v>70</v>
+      </c>
+      <c r="F49" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" t="s">
+        <v>97</v>
+      </c>
+      <c r="E50" t="s">
+        <v>76</v>
+      </c>
+      <c r="F50" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" t="s">
+        <v>97</v>
+      </c>
+      <c r="E51" t="s">
+        <v>77</v>
+      </c>
+      <c r="F51" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" t="s">
+        <v>97</v>
+      </c>
+      <c r="E52" t="s">
+        <v>78</v>
+      </c>
+      <c r="F52" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>39</v>
+      </c>
+      <c r="D53" t="s">
+        <v>97</v>
+      </c>
+      <c r="E53" t="s">
+        <v>79</v>
+      </c>
+      <c r="F53" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
+        <v>39</v>
+      </c>
+      <c r="D54" t="s">
+        <v>97</v>
+      </c>
+      <c r="E54" t="s">
+        <v>80</v>
+      </c>
+      <c r="F54" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>39</v>
+      </c>
+      <c r="D55" t="s">
+        <v>97</v>
+      </c>
+      <c r="E55" t="s">
+        <v>81</v>
+      </c>
+      <c r="F55" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>39</v>
+      </c>
+      <c r="D56" t="s">
+        <v>97</v>
+      </c>
+      <c r="E56" t="s">
+        <v>77</v>
+      </c>
+      <c r="F56" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" t="s">
+        <v>97</v>
+      </c>
+      <c r="E57" t="s">
+        <v>77</v>
+      </c>
+      <c r="F57" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" t="s">
+        <v>39</v>
+      </c>
+      <c r="D58" t="s">
+        <v>97</v>
+      </c>
+      <c r="E58" t="s">
+        <v>43</v>
+      </c>
+      <c r="F58" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>39</v>
+      </c>
+      <c r="D59" t="s">
+        <v>97</v>
+      </c>
+      <c r="E59" t="s">
+        <v>82</v>
+      </c>
+      <c r="F59" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>39</v>
+      </c>
+      <c r="D60" t="s">
+        <v>97</v>
+      </c>
+      <c r="E60" t="s">
+        <v>83</v>
+      </c>
+      <c r="F60" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61" t="s">
+        <v>39</v>
+      </c>
+      <c r="D61" t="s">
+        <v>97</v>
+      </c>
+      <c r="E61" t="s">
+        <v>60</v>
+      </c>
+      <c r="F61" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" t="s">
+        <v>39</v>
+      </c>
+      <c r="D62" t="s">
+        <v>97</v>
+      </c>
+      <c r="E62" t="s">
+        <v>40</v>
+      </c>
+      <c r="F62" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s">
+        <v>39</v>
+      </c>
+      <c r="D63" t="s">
+        <v>97</v>
+      </c>
+      <c r="E63" t="s">
+        <v>84</v>
+      </c>
+      <c r="F63" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s">
+        <v>39</v>
+      </c>
+      <c r="D64" t="s">
+        <v>97</v>
+      </c>
+      <c r="E64" t="s">
+        <v>40</v>
+      </c>
+      <c r="F64" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>2</v>
+      </c>
+      <c r="C65" t="s">
+        <v>39</v>
+      </c>
+      <c r="D65" t="s">
+        <v>97</v>
+      </c>
+      <c r="E65" t="s">
+        <v>85</v>
+      </c>
+      <c r="F65" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" t="s">
+        <v>39</v>
+      </c>
+      <c r="D66" t="s">
+        <v>97</v>
+      </c>
+      <c r="E66" t="s">
+        <v>52</v>
+      </c>
+      <c r="F66" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67" t="s">
+        <v>39</v>
+      </c>
+      <c r="D67" t="s">
+        <v>97</v>
+      </c>
+      <c r="E67" t="s">
+        <v>40</v>
+      </c>
+      <c r="F67" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" t="s">
+        <v>39</v>
+      </c>
+      <c r="D68" t="s">
+        <v>97</v>
+      </c>
+      <c r="E68" t="s">
+        <v>86</v>
+      </c>
+      <c r="F68" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" t="s">
+        <v>39</v>
+      </c>
+      <c r="D69" t="s">
+        <v>97</v>
+      </c>
+      <c r="E69" t="s">
+        <v>87</v>
+      </c>
+      <c r="F69" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" t="s">
+        <v>39</v>
+      </c>
+      <c r="D70" t="s">
+        <v>97</v>
+      </c>
+      <c r="E70" t="s">
+        <v>88</v>
+      </c>
+      <c r="F70" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>2</v>
+      </c>
+      <c r="C71" t="s">
+        <v>39</v>
+      </c>
+      <c r="D71" t="s">
+        <v>97</v>
+      </c>
+      <c r="E71" t="s">
+        <v>89</v>
+      </c>
+      <c r="F71" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" t="s">
+        <v>39</v>
+      </c>
+      <c r="D72" t="s">
+        <v>97</v>
+      </c>
+      <c r="E72" t="s">
+        <v>90</v>
+      </c>
+      <c r="F72" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s">
+        <v>39</v>
+      </c>
+      <c r="D73" t="s">
+        <v>97</v>
+      </c>
+      <c r="E73" t="s">
+        <v>91</v>
+      </c>
+      <c r="F73" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>2</v>
+      </c>
+      <c r="C74" t="s">
+        <v>39</v>
+      </c>
+      <c r="D74" t="s">
+        <v>97</v>
+      </c>
+      <c r="E74" t="s">
+        <v>92</v>
+      </c>
+      <c r="F74" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>2</v>
+      </c>
+      <c r="C75" t="s">
+        <v>39</v>
+      </c>
+      <c r="D75" t="s">
+        <v>97</v>
+      </c>
+      <c r="E75" t="s">
+        <v>93</v>
+      </c>
+      <c r="F75" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C76" t="s">
+        <v>39</v>
+      </c>
+      <c r="D76" t="s">
+        <v>97</v>
+      </c>
+      <c r="E76" t="s">
+        <v>94</v>
+      </c>
+      <c r="F76" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>2</v>
+      </c>
+      <c r="C77" t="s">
+        <v>39</v>
+      </c>
+      <c r="D77" t="s">
+        <v>97</v>
+      </c>
+      <c r="E77" t="s">
+        <v>95</v>
+      </c>
+      <c r="F77" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>2</v>
+      </c>
+      <c r="C78" t="s">
+        <v>39</v>
+      </c>
+      <c r="D78" t="s">
+        <v>97</v>
+      </c>
+      <c r="E78" t="s">
+        <v>96</v>
+      </c>
+      <c r="F78" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>